<commit_message>
Se completa la clase AsignacionNuevos | Se empieza con los tests de AsignacionNuevos
</commit_message>
<xml_diff>
--- a/output/results/recursosxcno_antiguos.xlsx
+++ b/output/results/recursosxcno_antiguos.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,24 +441,56 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>recursosxcno</t>
+          <t>ipo_ponderado</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>cuposxcno</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ipo</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>n_programas</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>participacion_ipo</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>recursosxcno</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>1231</v>
       </c>
       <c r="B2" t="n">
+        <v>96.55310409621252</v>
+      </c>
+      <c r="C2" t="n">
+        <v>200</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9655310409621252</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.08149173855568445</v>
+      </c>
+      <c r="G2" t="n">
         <v>107569094.8935035</v>
-      </c>
-      <c r="C2" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -466,10 +498,22 @@
         <v>1345</v>
       </c>
       <c r="B3" t="n">
+        <v>99.74631914374956</v>
+      </c>
+      <c r="C3" t="n">
+        <v>160</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.24682898929687</v>
+      </c>
+      <c r="E3" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.08418684243910454</v>
+      </c>
+      <c r="G3" t="n">
         <v>111126632.019618</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -477,10 +521,22 @@
         <v>2242</v>
       </c>
       <c r="B4" t="n">
+        <v>40.66875408474579</v>
+      </c>
+      <c r="C4" t="n">
+        <v>75</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.5422500544632771</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.03432481540890753</v>
+      </c>
+      <c r="G4" t="n">
         <v>45308756.33975793</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -488,10 +544,22 @@
         <v>2281</v>
       </c>
       <c r="B5" t="n">
+        <v>55.2338365446359</v>
+      </c>
+      <c r="C5" t="n">
+        <v>83</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.6654679101763361</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.04661788359116507</v>
+      </c>
+      <c r="G5" t="n">
         <v>61535606.34033789</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -499,10 +567,22 @@
         <v>3311</v>
       </c>
       <c r="B6" t="n">
+        <v>47.73412360227283</v>
+      </c>
+      <c r="C6" t="n">
+        <v>100</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.4773412360227283</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.04028805450837633</v>
+      </c>
+      <c r="G6" t="n">
         <v>53180231.95105676</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -510,10 +590,22 @@
         <v>3315</v>
       </c>
       <c r="B7" t="n">
+        <v>95.97906473146111</v>
+      </c>
+      <c r="C7" t="n">
+        <v>160</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.199738309143264</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0810072438698753</v>
+      </c>
+      <c r="G7" t="n">
         <v>106929561.9082354</v>
-      </c>
-      <c r="C7" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -521,10 +613,22 @@
         <v>4311</v>
       </c>
       <c r="B8" t="n">
+        <v>143.1970855311291</v>
+      </c>
+      <c r="C8" t="n">
+        <v>300</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1.43197085531129</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.120859702702158</v>
+      </c>
+      <c r="G8" t="n">
         <v>159534807.5668485</v>
-      </c>
-      <c r="C8" t="n">
-        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -532,10 +636,22 @@
         <v>5223</v>
       </c>
       <c r="B9" t="n">
+        <v>15.08304680655133</v>
+      </c>
+      <c r="C9" t="n">
+        <v>30</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.5027682268850443</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.01273023501924728</v>
+      </c>
+      <c r="G9" t="n">
         <v>16803910.2254064</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -543,10 +659,22 @@
         <v>6234</v>
       </c>
       <c r="B10" t="n">
+        <v>32.62370608853713</v>
+      </c>
+      <c r="C10" t="n">
+        <v>60</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.5437284348089521</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.02753471835183438</v>
+      </c>
+      <c r="G10" t="n">
         <v>36345828.22442139</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -554,10 +682,22 @@
         <v>6322</v>
       </c>
       <c r="B11" t="n">
+        <v>158.1962925708634</v>
+      </c>
+      <c r="C11" t="n">
+        <v>285</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.110149421549919</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.1335191761604801</v>
+      </c>
+      <c r="G11" t="n">
         <v>176245312.5318337</v>
-      </c>
-      <c r="C11" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -565,10 +705,22 @@
         <v>6355</v>
       </c>
       <c r="B12" t="n">
+        <v>194.070393492528</v>
+      </c>
+      <c r="C12" t="n">
+        <v>350</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2.217947354200319</v>
+      </c>
+      <c r="E12" t="n">
+        <v>4</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.1637972586788359</v>
+      </c>
+      <c r="G12" t="n">
         <v>216212381.4560634</v>
-      </c>
-      <c r="C12" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -576,10 +728,22 @@
         <v>8325</v>
       </c>
       <c r="B13" t="n">
+        <v>205.7350392827064</v>
+      </c>
+      <c r="C13" t="n">
+        <v>410</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2.508963893691542</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.1736423307143312</v>
+      </c>
+      <c r="G13" t="n">
         <v>229207876.5429172</v>
-      </c>
-      <c r="C13" t="n">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>